<commit_message>
insights from CAP curve
</commit_message>
<xml_diff>
--- a/CAP-Curve-Template copy.xlsx
+++ b/CAP-Curve-Template copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Cumulative Accuracy Profile" sheetId="1" r:id="rId1"/>
@@ -13072,11 +13072,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2099881568"/>
-        <c:axId val="-2099879248"/>
+        <c:axId val="235629536"/>
+        <c:axId val="268503936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2099881568"/>
+        <c:axId val="235629536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13086,7 +13086,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099879248"/>
+        <c:crossAx val="268503936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13094,9 +13094,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099879248"/>
+        <c:axId val="268503936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -13104,7 +13105,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099881568"/>
+        <c:crossAx val="235629536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13451,7 +13452,7 @@
   <dimension ref="A1:Q1007"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>